<commit_message>
Teste de Mesa Excel
</commit_message>
<xml_diff>
--- a/Exercício Teste de Mesa.xlsx
+++ b/Exercício Teste de Mesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Nova pasta\aula-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ABDCC6F-5CD4-42C9-A579-DD4BC1874DEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3601A6-8301-4FC3-9376-48F16AAD9E59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E34D1239-4496-4189-A6B3-EC748E69430F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Linha</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>